<commit_message>
updating with all names taken out
</commit_message>
<xml_diff>
--- a/LunchBuds.xlsx
+++ b/LunchBuds.xlsx
@@ -8,194 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoonsoonam/Documents/1USC 2022-2023/Extra Curricular /Scope/lunchBuds/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC880EB8-1FE7-7D49-A2AC-0B33AFEEAEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA97752-DD86-B445-A8F0-4FBD27D2D486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pairs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Names</t>
-  </si>
-  <si>
-    <t>Week 1</t>
-  </si>
-  <si>
-    <t>Isabella Paine</t>
-  </si>
-  <si>
-    <t>Vincent Li Ruan</t>
-  </si>
-  <si>
-    <t>Jenny Liu</t>
-  </si>
-  <si>
-    <t>Joshua Yoo</t>
-  </si>
-  <si>
-    <t>Phillip Suh</t>
-  </si>
-  <si>
-    <t>Stephanie Yu</t>
-  </si>
-  <si>
-    <t>Paul Somodi</t>
-  </si>
-  <si>
-    <t>Ethan Sawyer</t>
-  </si>
-  <si>
-    <t>Hallie Faust</t>
-  </si>
-  <si>
-    <t>Yoonsoo Nam</t>
-  </si>
-  <si>
-    <t>Edgar Patino</t>
-  </si>
-  <si>
-    <t>Ines Kim</t>
-  </si>
-  <si>
-    <t>Jake Kandell</t>
-  </si>
-  <si>
-    <t>Ethan Park</t>
-  </si>
-  <si>
-    <t>Gabriela Gutzmer</t>
-  </si>
-  <si>
-    <t>Nicole Russack </t>
-  </si>
-  <si>
-    <t>Ryan Lampotang</t>
-  </si>
-  <si>
-    <t>Nicole Russack</t>
-  </si>
-  <si>
-    <t>Anoushka Makkad</t>
-  </si>
-  <si>
-    <t>Neel Gupta</t>
-  </si>
-  <si>
-    <t>Serena Yang</t>
-  </si>
-  <si>
-    <t>Toby Fenner</t>
-  </si>
-  <si>
-    <t>Daniel Tadesse</t>
-  </si>
-  <si>
-    <t>Ju Lee</t>
-  </si>
-  <si>
-    <t>Leonel Herrera</t>
-  </si>
-  <si>
-    <t>Alex Nemzek</t>
-  </si>
-  <si>
-    <t>Crystal Okoli</t>
-  </si>
-  <si>
-    <t>AJ Mannan</t>
-  </si>
-  <si>
-    <t>Sarah Chen</t>
-  </si>
-  <si>
-    <t>Rhea Mehta</t>
-  </si>
-  <si>
-    <t>Aaron Shields</t>
-  </si>
-  <si>
-    <t>Mariana Avendano Herrera</t>
-  </si>
-  <si>
-    <t>Sahithi Lingampalli</t>
-  </si>
-  <si>
-    <t>John McCance</t>
-  </si>
-  <si>
-    <t>Iliyan Hariyani</t>
-  </si>
-  <si>
-    <t>Reese Bretow</t>
-  </si>
-  <si>
-    <t>Jadrian Tan</t>
-  </si>
-  <si>
-    <t>Nathan Lee</t>
-  </si>
-  <si>
-    <t>Brian Wagner</t>
-  </si>
-  <si>
-    <t>Shriya Upadhyay</t>
-  </si>
-  <si>
-    <t>Ellie Xing</t>
-  </si>
-  <si>
-    <t>Tanya Sankhla</t>
-  </si>
-  <si>
-    <t>Parini Gandhi</t>
-  </si>
-  <si>
-    <t>Hanyoung Kim</t>
-  </si>
-  <si>
-    <t>Obinna Obed</t>
-  </si>
-  <si>
-    <t>Ralph Jeanty</t>
-  </si>
-  <si>
-    <t>Adam Lehavi</t>
-  </si>
-  <si>
-    <t>Andrew Holt</t>
-  </si>
-  <si>
-    <t>Athena Diamantidis</t>
-  </si>
-  <si>
-    <t>Charlie Feuerborn</t>
-  </si>
-  <si>
-    <t>Daniel Zeng</t>
-  </si>
-  <si>
-    <t>Miru Jun</t>
-  </si>
-  <si>
-    <t>Will Farhat</t>
   </si>
 </sst>
 </file>
@@ -331,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -343,6 +170,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,31 +512,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="125" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="22" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
+      <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="F1" s="12"/>
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
@@ -715,16 +541,12 @@
       <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="F2" s="11"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
@@ -732,16 +554,12 @@
       <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="F3" s="11"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -749,16 +567,12 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="11"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -766,16 +580,12 @@
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="11"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -783,16 +593,12 @@
       <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="11"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -800,16 +606,12 @@
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="11"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -817,16 +619,12 @@
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>46</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="11"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -834,15 +632,11 @@
       <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="A9" s="9"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="F9" s="11"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -850,15 +644,11 @@
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="A10" s="10"/>
+      <c r="B10" s="8"/>
       <c r="C10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="11"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -866,15 +656,11 @@
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>7</v>
-      </c>
+      <c r="A11" s="10"/>
+      <c r="B11" s="8"/>
       <c r="C11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="11"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -882,15 +668,11 @@
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>30</v>
-      </c>
+      <c r="A12" s="10"/>
+      <c r="B12" s="8"/>
       <c r="C12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="11"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -898,15 +680,11 @@
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="A13" s="10"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="F13" s="11"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -914,15 +692,11 @@
       <c r="K13" s="1"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="A14" s="10"/>
+      <c r="B14" s="8"/>
       <c r="C14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="F14" s="11"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -930,15 +704,11 @@
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>36</v>
-      </c>
+      <c r="A15" s="10"/>
+      <c r="B15" s="8"/>
       <c r="C15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="F15" s="11"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -946,15 +716,11 @@
       <c r="K15" s="1"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>15</v>
-      </c>
+      <c r="A16" s="10"/>
+      <c r="B16" s="8"/>
       <c r="C16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="F16" s="11"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -962,15 +728,11 @@
       <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>37</v>
-      </c>
+      <c r="A17" s="10"/>
+      <c r="B17" s="8"/>
       <c r="C17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="F17" s="11"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -978,15 +740,11 @@
       <c r="K17" s="1"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>24</v>
-      </c>
+      <c r="A18" s="10"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+      <c r="F18" s="11"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -994,15 +752,11 @@
       <c r="K18" s="1"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="A19" s="10"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="F19" s="11"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -1010,15 +764,11 @@
       <c r="K19" s="1"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>8</v>
-      </c>
+      <c r="A20" s="10"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
+      <c r="F20" s="11"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -1026,15 +776,11 @@
       <c r="K20" s="1"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>22</v>
-      </c>
+      <c r="A21" s="10"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="11"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -1042,15 +788,11 @@
       <c r="K21" s="1"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>45</v>
-      </c>
+      <c r="A22" s="10"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="F22" s="11"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1058,15 +800,11 @@
       <c r="K22" s="1"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>54</v>
-      </c>
+      <c r="A23" s="10"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="F23" s="11"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -1074,15 +812,11 @@
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="A24" s="10"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="F24" s="11"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -1090,15 +824,11 @@
       <c r="K24" s="1"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>29</v>
-      </c>
+      <c r="A25" s="10"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="F25" s="11"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -1106,15 +836,11 @@
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>53</v>
-      </c>
+      <c r="A26" s="10"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="F26" s="11"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -1122,15 +848,11 @@
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>48</v>
-      </c>
+      <c r="A27" s="10"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="F27" s="11"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -1138,15 +860,11 @@
       <c r="K27" s="1"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>2</v>
-      </c>
+      <c r="A28" s="10"/>
+      <c r="B28" s="8"/>
       <c r="C28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
+      <c r="F28" s="11"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -1154,15 +872,11 @@
       <c r="K28" s="1"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>6</v>
-      </c>
+      <c r="A29" s="10"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
+      <c r="F29" s="11"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -1170,15 +884,11 @@
       <c r="K29" s="1"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>18</v>
-      </c>
+      <c r="A30" s="10"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+      <c r="F30" s="11"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -1186,15 +896,11 @@
       <c r="K30" s="1"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>50</v>
-      </c>
+      <c r="A31" s="10"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="F31" s="11"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -1202,15 +908,11 @@
       <c r="K31" s="1"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>14</v>
-      </c>
+      <c r="A32" s="10"/>
+      <c r="B32" s="8"/>
       <c r="C32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+      <c r="F32" s="11"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
@@ -1218,15 +920,11 @@
       <c r="K32" s="1"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="A33" s="10"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
+      <c r="F33" s="11"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
@@ -1234,15 +932,11 @@
       <c r="K33" s="1"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="A34" s="10"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="F34" s="11"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
@@ -1250,15 +944,11 @@
       <c r="K34" s="1"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>2</v>
-      </c>
+      <c r="A35" s="10"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
+      <c r="F35" s="11"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
@@ -1266,15 +956,11 @@
       <c r="K35" s="1"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>39</v>
-      </c>
+      <c r="A36" s="10"/>
+      <c r="B36" s="8"/>
       <c r="C36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
+      <c r="F36" s="11"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
@@ -1282,15 +968,11 @@
       <c r="K36" s="1"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>5</v>
-      </c>
+      <c r="A37" s="10"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
+      <c r="F37" s="11"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
@@ -1298,15 +980,11 @@
       <c r="K37" s="1"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="A38" s="10"/>
+      <c r="B38" s="8"/>
       <c r="C38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
+      <c r="F38" s="11"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
@@ -1314,15 +992,11 @@
       <c r="K38" s="1"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="A39" s="10"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="1"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
+      <c r="F39" s="11"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
@@ -1330,15 +1004,11 @@
       <c r="K39" s="1"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>52</v>
-      </c>
+      <c r="A40" s="10"/>
+      <c r="B40" s="8"/>
       <c r="C40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
+      <c r="F40" s="11"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -1346,15 +1016,11 @@
       <c r="K40" s="1"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B41" s="8" t="s">
-        <v>51</v>
-      </c>
+      <c r="A41" s="10"/>
+      <c r="B41" s="8"/>
       <c r="C41" s="1"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
+      <c r="F41" s="11"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
@@ -1362,15 +1028,11 @@
       <c r="K41" s="1"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="A42" s="10"/>
+      <c r="B42" s="8"/>
       <c r="C42" s="1"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
+      <c r="F42" s="11"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
@@ -1378,15 +1040,11 @@
       <c r="K42" s="1"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>4</v>
-      </c>
+      <c r="A43" s="10"/>
+      <c r="B43" s="8"/>
       <c r="C43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
+      <c r="F43" s="11"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
@@ -1394,15 +1052,11 @@
       <c r="K43" s="1"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>17</v>
-      </c>
+      <c r="A44" s="10"/>
+      <c r="B44" s="8"/>
       <c r="C44" s="1"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
+      <c r="F44" s="11"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
@@ -1410,15 +1064,11 @@
       <c r="K44" s="1"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>16</v>
-      </c>
+      <c r="A45" s="10"/>
+      <c r="B45" s="8"/>
       <c r="C45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
+      <c r="F45" s="11"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -1426,15 +1076,11 @@
       <c r="K45" s="1"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>49</v>
-      </c>
+      <c r="A46" s="10"/>
+      <c r="B46" s="8"/>
       <c r="C46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
+      <c r="F46" s="11"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
@@ -1442,15 +1088,11 @@
       <c r="K46" s="1"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="A47" s="10"/>
+      <c r="B47" s="8"/>
       <c r="C47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
+      <c r="F47" s="11"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
@@ -1458,15 +1100,11 @@
       <c r="K47" s="1"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>41</v>
-      </c>
+      <c r="A48" s="10"/>
+      <c r="B48" s="8"/>
       <c r="C48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
+      <c r="F48" s="11"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
@@ -1474,15 +1112,11 @@
       <c r="K48" s="1"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="A49" s="10"/>
+      <c r="B49" s="8"/>
       <c r="C49" s="1"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
+      <c r="F49" s="11"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
@@ -1490,15 +1124,11 @@
       <c r="K49" s="1"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>11</v>
-      </c>
+      <c r="A50" s="10"/>
+      <c r="B50" s="8"/>
       <c r="C50" s="1"/>
       <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
+      <c r="F50" s="11"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -1506,15 +1136,11 @@
       <c r="K50" s="1"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="A51" s="10"/>
+      <c r="B51" s="8"/>
       <c r="C51" s="1"/>
       <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
+      <c r="F51" s="11"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
@@ -1522,20 +1148,16 @@
       <c r="K51" s="1"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="A52" s="10"/>
+      <c r="B52" s="8"/>
       <c r="C52" s="1"/>
+      <c r="F52" s="11"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="A53" s="10"/>
       <c r="B53" s="8"/>
       <c r="C53" s="1"/>
+      <c r="F53" s="11"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B54" s="8"/>

</xml_diff>